<commit_message>
Per que s'entengui millor
</commit_message>
<xml_diff>
--- a/Estimacion horas.xlsx
+++ b/Estimacion horas.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\Documents\GitHub\Samurai-Shodown-Neo-Geo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Albert</t>
   </si>
@@ -66,13 +61,22 @@
   </si>
   <si>
     <t>300 minuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Background del mapa de Haohamru(con todas sus animaciones)</t>
+  </si>
+  <si>
+    <t>Crear modulos menu y VictoryHaohmaru, y backgrounds</t>
+  </si>
+  <si>
+    <t>45 minuts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +196,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -211,6 +224,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -218,24 +240,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -525,27 +529,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="4" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>3</v>
@@ -557,11 +561,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="21" t="s">
@@ -571,213 +575,212 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
-      <c r="B5" s="13"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="22"/>
       <c r="D5" s="25"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
-      <c r="B6" s="14"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="23"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="12">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="20"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="9"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="19"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="20"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="12">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="10"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="20"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="14"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="12">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="15"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="10"/>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1"/>
       <c r="B21" s="17"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="11"/>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="12">
         <v>420</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="19"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="20"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="11"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="15"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="9"/>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1"/>
       <c r="B29" s="16"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="10"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="10"/>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1"/>
       <c r="B30" s="17"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B19:B21"/>
@@ -792,6 +795,19 @@
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix jump and punch
</commit_message>
<xml_diff>
--- a/Estimacion horas.xlsx
+++ b/Estimacion horas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albertgb7\Documents\GitHub\Samurai-Shodown-Neo-Geo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Samurai-Shodown-Neo-Geo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Albert</t>
   </si>
@@ -81,12 +81,15 @@
   </si>
   <si>
     <t>modulo proyectiles, animacion proyectil, colliders</t>
+  </si>
+  <si>
+    <t>Arreglar puñetazo y salto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -276,75 +279,75 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,7 +409,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,7 +444,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -629,7 +632,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D21"/>
+      <selection activeCell="D19" sqref="D19:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,25 +644,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="N1" s="38"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="N1" s="18"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="38"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -697,13 +700,13 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="43">
         <v>60</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -729,9 +732,9 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="34"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="44"/>
       <c r="F5" s="1"/>
       <c r="G5" s="16"/>
       <c r="H5" s="10"/>
@@ -743,8 +746,8 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="5"/>
       <c r="F6" s="1"/>
       <c r="G6" s="17"/>
@@ -757,7 +760,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="37" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="27" t="s">
@@ -769,7 +772,7 @@
       <c r="F7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="24" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="27" t="s">
@@ -781,27 +784,27 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="22"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="28"/>
       <c r="D8" s="31"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="36"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="28"/>
       <c r="I8" s="31"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="23"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="29"/>
       <c r="D9" s="32"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="37"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="29"/>
       <c r="I9" s="32"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="27" t="s">
@@ -822,11 +825,11 @@
       <c r="I10" s="12">
         <v>70</v>
       </c>
-      <c r="L10" s="38"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="22"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="28"/>
       <c r="D11" s="31"/>
       <c r="F11" s="1"/>
@@ -836,7 +839,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="23"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="29"/>
       <c r="D12" s="32"/>
       <c r="F12" s="1"/>
@@ -846,7 +849,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="27" t="s">
@@ -856,33 +859,33 @@
         <v>270</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="35"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="27"/>
       <c r="I13" s="30"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="22"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="28"/>
       <c r="D14" s="31"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="36"/>
+      <c r="G14" s="25"/>
       <c r="H14" s="28"/>
       <c r="I14" s="31"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="23"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="29"/>
       <c r="D15" s="32"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="37"/>
+      <c r="G15" s="26"/>
       <c r="H15" s="29"/>
       <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="37" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="27" t="s">
@@ -892,171 +895,146 @@
         <v>90</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="35"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="27"/>
       <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="22"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="28"/>
       <c r="D17" s="31"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="36"/>
+      <c r="G17" s="25"/>
       <c r="H17" s="28"/>
       <c r="I17" s="31"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="23"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="29"/>
       <c r="D18" s="32"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="43"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="33"/>
       <c r="H18" s="29"/>
       <c r="I18" s="32"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="30"/>
+      <c r="B19" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="30">
+        <v>40</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="25"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="28"/>
       <c r="D20" s="31"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="35"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="27"/>
       <c r="I20" s="30"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="26"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="29"/>
       <c r="D21" s="32"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="36"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="28"/>
       <c r="I21" s="31"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="21"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="27"/>
       <c r="D22" s="30"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="37"/>
+      <c r="G22" s="26"/>
       <c r="H22" s="29"/>
       <c r="I22" s="32"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="22"/>
+      <c r="B23" s="38"/>
       <c r="C23" s="28"/>
       <c r="D23" s="31"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="35"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="27"/>
       <c r="I23" s="30"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="23"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="29"/>
       <c r="D24" s="32"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="36"/>
+      <c r="G24" s="25"/>
       <c r="H24" s="28"/>
       <c r="I24" s="31"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="35"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="27"/>
       <c r="D25" s="30"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="37"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="29"/>
       <c r="I25" s="32"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="36"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="28"/>
       <c r="D26" s="31"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="35"/>
+      <c r="G26" s="24"/>
       <c r="H26" s="27"/>
       <c r="I26" s="30"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="37"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="29"/>
       <c r="D27" s="32"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="36"/>
+      <c r="G27" s="25"/>
       <c r="H27" s="28"/>
       <c r="I27" s="31"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="24"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="27"/>
       <c r="D28" s="30"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="37"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="29"/>
       <c r="I28" s="32"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="25"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="28"/>
       <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="26"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="29"/>
       <c r="D30" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="I26:I28"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B19:B21"/>
@@ -1071,6 +1049,37 @@
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="I26:I28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>